<commit_message>
Felder waren veraltet -> update
</commit_message>
<xml_diff>
--- a/data/dataSets/dataSets.xlsx
+++ b/data/dataSets/dataSets.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>description.de</t>
   </si>
@@ -78,28 +78,34 @@
     <t>language</t>
   </si>
   <si>
-    <t>numberOfAnalyzedVariables</t>
-  </si>
-  <si>
     <t>gsl2008_o_1-0-0</t>
   </si>
   <si>
     <t>gsl2008_r_1-0-0</t>
   </si>
   <si>
-    <t>DZHW-Studienberechtigtenpanel 2008 - Personendatensatz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DZHW Panel Study of School Leavers 2008 - Individual data </t>
-  </si>
-  <si>
-    <t>DZHW Panel Study of School Leavers 2008 - Individual data</t>
-  </si>
-  <si>
     <t>Personendatensatz des DZHW-Studienberechtigtenpanels 2008</t>
   </si>
   <si>
     <t>Individual data of the DZHW Panel Study of School Leavers 2008</t>
+  </si>
+  <si>
+    <t>Kann über Remote Desktop genutzt werden</t>
+  </si>
+  <si>
+    <t>can be used via remote desktop</t>
+  </si>
+  <si>
+    <t>Ist am Gastwissenschaftlerarbeitsplatz im DZHW in Hannover verfügbar</t>
+  </si>
+  <si>
+    <t>available at the workspace for visiting scientists at the DZHW in Hannover</t>
+  </si>
+  <si>
+    <t>breit</t>
+  </si>
+  <si>
+    <t>wide</t>
   </si>
 </sst>
 </file>
@@ -109,7 +115,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;[$€-407];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-407]"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -168,6 +174,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -206,7 +219,7 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -221,6 +234,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -534,7 +554,7 @@
   <dimension ref="A1:H1582"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,14 +587,14 @@
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>7</v>
+      <c r="F1" t="s">
+        <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
-      <c r="H1" t="s">
-        <v>14</v>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -582,10 +602,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -594,8 +614,24 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G8" s="2"/>
@@ -5330,24 +5366,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.42578125" customWidth="1"/>
     <col min="5" max="5" width="34.42578125" customWidth="1"/>
     <col min="6" max="6" width="46.5703125" customWidth="1"/>
     <col min="7" max="1026" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -5355,85 +5391,63 @@
         <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="G1" s="4"/>
       <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="4">
         <v>32621</v>
       </c>
-      <c r="C2" s="4">
-        <v>1165</v>
+      <c r="C2" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>23</v>
+      <c r="E2" s="10" t="s">
+        <v>27</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2">
+      <c r="F2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="4">
         <v>32621</v>
       </c>
-      <c r="C3" s="4">
-        <v>1100</v>
+      <c r="C3" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="G3">
+      <c r="F3">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="1"/>
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="7"/>
+      <c r="F4" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>